<commit_message>
Add methodology narrative and publish pollster MAE-based weights on dashboard
</commit_message>
<xml_diff>
--- a/codex_handoff_pack/outputs/weighted_time_series.xlsx
+++ b/codex_handoff_pack/outputs/weighted_time_series.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="weighted_time_series" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="weights" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4706,4 +4707,189 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>조사기관</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mae</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>weight_pct</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>리서치앤리서치</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1.715165533504263</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1852563467633035</v>
+      </c>
+      <c r="D2" t="n">
+        <v>18.52563467633035</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>엠브레인퍼블릭</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.988068392353487</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1598261418236138</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15.98261418236138</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>리서치뷰</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2.520935456058236</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1260426164691112</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12.60426164691112</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>에이스리서치</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2.706784148984008</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1173884888274516</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11.73884888274516</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>한국리서치</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.984805325724369</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.106454279645263</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10.6454279645263</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>조원씨앤아이</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3.005944774053744</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1057056349052044</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10.57056349052044</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>알앤써치</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.15182333959994</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.07653150792826108</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7.653150792826108</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>리얼미터</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.376554982336593</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0726016929100001</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.26016929100001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>코리아리서치인터내셔널</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6.330433733753978</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.05019329072779152</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5.019329072779152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add weekly poll update runner with web-verified point + bias-adjusted fallback estimates
</commit_message>
<xml_diff>
--- a/codex_handoff_pack/outputs/weighted_time_series.xlsx
+++ b/codex_handoff_pack/outputs/weighted_time_series.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4702,6 +4702,38 @@
       </c>
       <c r="J133" t="n">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>46068</v>
+      </c>
+      <c r="B134" t="n">
+        <v>9</v>
+      </c>
+      <c r="C134" t="n">
+        <v>44.05515639839154</v>
+      </c>
+      <c r="D134" t="n">
+        <v>34.37801908529156</v>
+      </c>
+      <c r="E134" t="n">
+        <v>3.075842306832621</v>
+      </c>
+      <c r="F134" t="n">
+        <v>1.408262200504596</v>
+      </c>
+      <c r="G134" t="n">
+        <v>3.06674971272188</v>
+      </c>
+      <c r="H134" t="n">
+        <v>3.110334741159372</v>
+      </c>
+      <c r="I134" t="n">
+        <v>9.642987088043844</v>
+      </c>
+      <c r="J134" t="n">
+        <v>1.262648467054583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add NESDC weekly attachment fetch/apply workflow with xlsx-first update path
</commit_message>
<xml_diff>
--- a/codex_handoff_pack/outputs/weighted_time_series.xlsx
+++ b/codex_handoff_pack/outputs/weighted_time_series.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4702,38 +4702,6 @@
       </c>
       <c r="J133" t="n">
         <v>0.7</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="2" t="n">
-        <v>46068</v>
-      </c>
-      <c r="B134" t="n">
-        <v>9</v>
-      </c>
-      <c r="C134" t="n">
-        <v>44.05515639839154</v>
-      </c>
-      <c r="D134" t="n">
-        <v>34.37801908529156</v>
-      </c>
-      <c r="E134" t="n">
-        <v>3.075842306832621</v>
-      </c>
-      <c r="F134" t="n">
-        <v>1.408262200504596</v>
-      </c>
-      <c r="G134" t="n">
-        <v>3.06674971272188</v>
-      </c>
-      <c r="H134" t="n">
-        <v>3.110334741159372</v>
-      </c>
-      <c r="I134" t="n">
-        <v>9.642987088043844</v>
-      </c>
-      <c r="J134" t="n">
-        <v>1.262648467054583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: hourly poll update (2026-02-16~2026-02-22)
</commit_message>
<xml_diff>
--- a/codex_handoff_pack/outputs/weighted_time_series.xlsx
+++ b/codex_handoff_pack/outputs/weighted_time_series.xlsx
@@ -21,16 +21,13 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -41,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -49,21 +46,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -430,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,53 +427,53 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>date_end</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>n_polls</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>더불어민주당</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>국민의힘</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>조국혁신당</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>진보당</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>개혁신당</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>기타정당</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>지지정당
 없음</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>모름/
 무응답</t>
@@ -493,7 +481,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="B2" t="n">
@@ -525,7 +513,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="1" t="n">
         <v>45660</v>
       </c>
       <c r="B3" t="n">
@@ -557,7 +545,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>45663</v>
       </c>
       <c r="B4" t="n">
@@ -589,7 +577,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="1" t="n">
         <v>45666</v>
       </c>
       <c r="B5" t="n">
@@ -621,7 +609,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="1" t="n">
         <v>45667</v>
       </c>
       <c r="B6" t="n">
@@ -653,7 +641,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="1" t="n">
         <v>45670</v>
       </c>
       <c r="B7" t="n">
@@ -685,7 +673,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="1" t="n">
         <v>45672</v>
       </c>
       <c r="B8" t="n">
@@ -717,7 +705,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="1" t="n">
         <v>45674</v>
       </c>
       <c r="B9" t="n">
@@ -749,7 +737,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="1" t="n">
         <v>45676</v>
       </c>
       <c r="B10" t="n">
@@ -779,7 +767,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="1" t="n">
         <v>45677</v>
       </c>
       <c r="B11" t="n">
@@ -811,7 +799,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="1" t="n">
         <v>45679</v>
       </c>
       <c r="B12" t="n">
@@ -843,7 +831,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="1" t="n">
         <v>45680</v>
       </c>
       <c r="B13" t="n">
@@ -875,7 +863,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="1" t="n">
         <v>45681</v>
       </c>
       <c r="B14" t="n">
@@ -907,7 +895,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="1" t="n">
         <v>45683</v>
       </c>
       <c r="B15" t="n">
@@ -939,7 +927,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="1" t="n">
         <v>45685</v>
       </c>
       <c r="B16" t="n">
@@ -971,7 +959,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="1" t="n">
         <v>45688</v>
       </c>
       <c r="B17" t="n">
@@ -1003,7 +991,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="1" t="n">
         <v>45690</v>
       </c>
       <c r="B18" t="n">
@@ -1035,7 +1023,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="1" t="n">
         <v>45691</v>
       </c>
       <c r="B19" t="n">
@@ -1067,7 +1055,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="1" t="n">
         <v>45694</v>
       </c>
       <c r="B20" t="n">
@@ -1099,7 +1087,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="1" t="n">
         <v>45695</v>
       </c>
       <c r="B21" t="n">
@@ -1131,7 +1119,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="1" t="n">
         <v>45698</v>
       </c>
       <c r="B22" t="n">
@@ -1163,7 +1151,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="1" t="n">
         <v>45701</v>
       </c>
       <c r="B23" t="n">
@@ -1195,7 +1183,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="1" t="n">
         <v>45702</v>
       </c>
       <c r="B24" t="n">
@@ -1227,7 +1215,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="1" t="n">
         <v>45705</v>
       </c>
       <c r="B25" t="n">
@@ -1259,7 +1247,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="1" t="n">
         <v>45708</v>
       </c>
       <c r="B26" t="n">
@@ -1291,7 +1279,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="1" t="n">
         <v>45709</v>
       </c>
       <c r="B27" t="n">
@@ -1323,7 +1311,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="1" t="n">
         <v>45712</v>
       </c>
       <c r="B28" t="n">
@@ -1355,7 +1343,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="1" t="n">
         <v>45716</v>
       </c>
       <c r="B29" t="n">
@@ -1387,7 +1375,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="1" t="n">
         <v>45719</v>
       </c>
       <c r="B30" t="n">
@@ -1419,7 +1407,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="1" t="n">
         <v>45720</v>
       </c>
       <c r="B31" t="n">
@@ -1451,7 +1439,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="1" t="n">
         <v>45723</v>
       </c>
       <c r="B32" t="n">
@@ -1483,7 +1471,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="1" t="n">
         <v>45726</v>
       </c>
       <c r="B33" t="n">
@@ -1515,7 +1503,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="1" t="n">
         <v>45730</v>
       </c>
       <c r="B34" t="n">
@@ -1547,7 +1535,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="1" t="n">
         <v>45732</v>
       </c>
       <c r="B35" t="n">
@@ -1579,7 +1567,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="1" t="n">
         <v>45733</v>
       </c>
       <c r="B36" t="n">
@@ -1611,7 +1599,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="1" t="n">
         <v>45737</v>
       </c>
       <c r="B37" t="n">
@@ -1643,7 +1631,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="1" t="n">
         <v>45740</v>
       </c>
       <c r="B38" t="n">
@@ -1675,7 +1663,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="1" t="n">
         <v>45744</v>
       </c>
       <c r="B39" t="n">
@@ -1707,7 +1695,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="1" t="n">
         <v>45747</v>
       </c>
       <c r="B40" t="n">
@@ -1739,7 +1727,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="1" t="n">
         <v>45751</v>
       </c>
       <c r="B41" t="n">
@@ -1771,7 +1759,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="1" t="n">
         <v>45752</v>
       </c>
       <c r="B42" t="n">
@@ -1801,7 +1789,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="1" t="n">
         <v>45754</v>
       </c>
       <c r="B43" t="n">
@@ -1831,7 +1819,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="1" t="n">
         <v>45756</v>
       </c>
       <c r="B44" t="n">
@@ -1863,7 +1851,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="1" t="n">
         <v>45757</v>
       </c>
       <c r="B45" t="n">
@@ -1895,7 +1883,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="1" t="n">
         <v>45758</v>
       </c>
       <c r="B46" t="n">
@@ -1927,7 +1915,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="1" t="n">
         <v>45759</v>
       </c>
       <c r="B47" t="n">
@@ -1959,7 +1947,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="1" t="n">
         <v>45760</v>
       </c>
       <c r="B48" t="n">
@@ -1989,7 +1977,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="1" t="n">
         <v>45761</v>
       </c>
       <c r="B49" t="n">
@@ -2021,7 +2009,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="1" t="n">
         <v>45765</v>
       </c>
       <c r="B50" t="n">
@@ -2053,7 +2041,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="1" t="n">
         <v>45767</v>
       </c>
       <c r="B51" t="n">
@@ -2085,7 +2073,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="1" t="n">
         <v>45768</v>
       </c>
       <c r="B52" t="n">
@@ -2115,7 +2103,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="1" t="n">
         <v>45770</v>
       </c>
       <c r="B53" t="n">
@@ -2147,7 +2135,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="1" t="n">
         <v>45771</v>
       </c>
       <c r="B54" t="n">
@@ -2179,7 +2167,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="1" t="n">
         <v>45772</v>
       </c>
       <c r="B55" t="n">
@@ -2211,7 +2199,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="1" t="n">
         <v>45773</v>
       </c>
       <c r="B56" t="n">
@@ -2243,7 +2231,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="1" t="n">
         <v>45774</v>
       </c>
       <c r="B57" t="n">
@@ -2275,7 +2263,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="1" t="n">
         <v>45781</v>
       </c>
       <c r="B58" t="n">
@@ -2307,7 +2295,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="1" t="n">
         <v>45782</v>
       </c>
       <c r="B59" t="n">
@@ -2339,7 +2327,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="1" t="n">
         <v>45784</v>
       </c>
       <c r="B60" t="n">
@@ -2371,7 +2359,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="1" t="n">
         <v>45785</v>
       </c>
       <c r="B61" t="n">
@@ -2403,7 +2391,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="1" t="n">
         <v>45786</v>
       </c>
       <c r="B62" t="n">
@@ -2435,7 +2423,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="1" t="n">
         <v>45789</v>
       </c>
       <c r="B63" t="n">
@@ -2465,7 +2453,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="1" t="n">
         <v>45790</v>
       </c>
       <c r="B64" t="n">
@@ -2497,7 +2485,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="1" t="n">
         <v>45791</v>
       </c>
       <c r="B65" t="n">
@@ -2529,7 +2517,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="1" t="n">
         <v>45792</v>
       </c>
       <c r="B66" t="n">
@@ -2561,7 +2549,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="1" t="n">
         <v>45793</v>
       </c>
       <c r="B67" t="n">
@@ -2593,7 +2581,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="1" t="n">
         <v>45796</v>
       </c>
       <c r="B68" t="n">
@@ -2625,7 +2613,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="1" t="n">
         <v>45797</v>
       </c>
       <c r="B69" t="n">
@@ -2657,7 +2645,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="1" t="n">
         <v>45798</v>
       </c>
       <c r="B70" t="n">
@@ -2689,7 +2677,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="1" t="n">
         <v>45799</v>
       </c>
       <c r="B71" t="n">
@@ -2721,7 +2709,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="1" t="n">
         <v>45800</v>
       </c>
       <c r="B72" t="n">
@@ -2753,7 +2741,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="1" t="n">
         <v>45802</v>
       </c>
       <c r="B73" t="n">
@@ -2785,7 +2773,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="1" t="n">
         <v>45804</v>
       </c>
       <c r="B74" t="n">
@@ -2817,7 +2805,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="1" t="n">
         <v>45813</v>
       </c>
       <c r="B75" t="n">
@@ -2849,7 +2837,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="1" t="n">
         <v>45821</v>
       </c>
       <c r="B76" t="n">
@@ -2881,7 +2869,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="1" t="n">
         <v>45828</v>
       </c>
       <c r="B77" t="n">
@@ -2913,7 +2901,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="1" t="n">
         <v>45835</v>
       </c>
       <c r="B78" t="n">
@@ -2945,7 +2933,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="1" t="n">
         <v>45838</v>
       </c>
       <c r="B79" t="n">
@@ -2977,7 +2965,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="1" t="n">
         <v>45842</v>
       </c>
       <c r="B80" t="n">
@@ -3009,7 +2997,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="1" t="n">
         <v>45845</v>
       </c>
       <c r="B81" t="n">
@@ -3041,7 +3029,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="1" t="n">
         <v>45849</v>
       </c>
       <c r="B82" t="n">
@@ -3073,7 +3061,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="1" t="n">
         <v>45856</v>
       </c>
       <c r="B83" t="n">
@@ -3105,7 +3093,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="1" t="n">
         <v>45859</v>
       </c>
       <c r="B84" t="n">
@@ -3137,7 +3125,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="1" t="n">
         <v>45863</v>
       </c>
       <c r="B85" t="n">
@@ -3169,7 +3157,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="1" t="n">
         <v>45866</v>
       </c>
       <c r="B86" t="n">
@@ -3201,7 +3189,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="1" t="n">
         <v>45869</v>
       </c>
       <c r="B87" t="n">
@@ -3233,7 +3221,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="1" t="n">
         <v>45873</v>
       </c>
       <c r="B88" t="n">
@@ -3265,7 +3253,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="1" t="n">
         <v>45877</v>
       </c>
       <c r="B89" t="n">
@@ -3297,7 +3285,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="1" t="n">
         <v>45883</v>
       </c>
       <c r="B90" t="n">
@@ -3329,7 +3317,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="1" t="n">
         <v>45887</v>
       </c>
       <c r="B91" t="n">
@@ -3361,7 +3349,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="1" t="n">
         <v>45891</v>
       </c>
       <c r="B92" t="n">
@@ -3393,7 +3381,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="1" t="n">
         <v>45898</v>
       </c>
       <c r="B93" t="n">
@@ -3425,7 +3413,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="1" t="n">
         <v>45900</v>
       </c>
       <c r="B94" t="n">
@@ -3457,7 +3445,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="1" t="n">
         <v>45905</v>
       </c>
       <c r="B95" t="n">
@@ -3489,7 +3477,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="1" t="n">
         <v>45910</v>
       </c>
       <c r="B96" t="n">
@@ -3521,7 +3509,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="1" t="n">
         <v>45912</v>
       </c>
       <c r="B97" t="n">
@@ -3553,7 +3541,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="1" t="n">
         <v>45915</v>
       </c>
       <c r="B98" t="n">
@@ -3585,7 +3573,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="1" t="n">
         <v>45919</v>
       </c>
       <c r="B99" t="n">
@@ -3617,7 +3605,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="1" t="n">
         <v>45926</v>
       </c>
       <c r="B100" t="n">
@@ -3649,7 +3637,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="1" t="n">
         <v>45929</v>
       </c>
       <c r="B101" t="n">
@@ -3681,7 +3669,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="n">
+      <c r="A102" s="1" t="n">
         <v>45930</v>
       </c>
       <c r="B102" t="n">
@@ -3713,7 +3701,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="n">
+      <c r="A103" s="1" t="n">
         <v>45932</v>
       </c>
       <c r="B103" t="n">
@@ -3745,7 +3733,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="n">
+      <c r="A104" s="1" t="n">
         <v>45947</v>
       </c>
       <c r="B104" t="n">
@@ -3777,7 +3765,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="n">
+      <c r="A105" s="1" t="n">
         <v>45950</v>
       </c>
       <c r="B105" t="n">
@@ -3809,7 +3797,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="n">
+      <c r="A106" s="1" t="n">
         <v>45954</v>
       </c>
       <c r="B106" t="n">
@@ -3841,7 +3829,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="n">
+      <c r="A107" s="1" t="n">
         <v>45961</v>
       </c>
       <c r="B107" t="n">
@@ -3873,7 +3861,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="n">
+      <c r="A108" s="1" t="n">
         <v>45964</v>
       </c>
       <c r="B108" t="n">
@@ -3905,7 +3893,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="n">
+      <c r="A109" s="1" t="n">
         <v>45968</v>
       </c>
       <c r="B109" t="n">
@@ -3937,7 +3925,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="n">
+      <c r="A110" s="1" t="n">
         <v>45975</v>
       </c>
       <c r="B110" t="n">
@@ -3969,7 +3957,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="n">
+      <c r="A111" s="1" t="n">
         <v>45978</v>
       </c>
       <c r="B111" t="n">
@@ -4001,7 +3989,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="n">
+      <c r="A112" s="1" t="n">
         <v>45982</v>
       </c>
       <c r="B112" t="n">
@@ -4033,7 +4021,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="n">
+      <c r="A113" s="1" t="n">
         <v>45989</v>
       </c>
       <c r="B113" t="n">
@@ -4065,7 +4053,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="n">
+      <c r="A114" s="1" t="n">
         <v>45991</v>
       </c>
       <c r="B114" t="n">
@@ -4097,7 +4085,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="n">
+      <c r="A115" s="1" t="n">
         <v>45996</v>
       </c>
       <c r="B115" t="n">
@@ -4129,7 +4117,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="n">
+      <c r="A116" s="1" t="n">
         <v>46003</v>
       </c>
       <c r="B116" t="n">
@@ -4161,7 +4149,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="n">
+      <c r="A117" s="1" t="n">
         <v>46006</v>
       </c>
       <c r="B117" t="n">
@@ -4193,7 +4181,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="n">
+      <c r="A118" s="1" t="n">
         <v>46010</v>
       </c>
       <c r="B118" t="n">
@@ -4225,7 +4213,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="n">
+      <c r="A119" s="1" t="n">
         <v>46017</v>
       </c>
       <c r="B119" t="n">
@@ -4257,7 +4245,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="n">
+      <c r="A120" s="1" t="n">
         <v>46019</v>
       </c>
       <c r="B120" t="n">
@@ -4289,7 +4277,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="n">
+      <c r="A121" s="1" t="n">
         <v>46020</v>
       </c>
       <c r="B121" t="n">
@@ -4321,7 +4309,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="n">
+      <c r="A122" s="1" t="n">
         <v>46021</v>
       </c>
       <c r="B122" t="n">
@@ -4353,7 +4341,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="n">
+      <c r="A123" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="B123" t="n">
@@ -4385,7 +4373,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="2" t="n">
+      <c r="A124" s="1" t="n">
         <v>46024</v>
       </c>
       <c r="B124" t="n">
@@ -4417,7 +4405,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="n">
+      <c r="A125" s="1" t="n">
         <v>46029</v>
       </c>
       <c r="B125" t="n">
@@ -4449,7 +4437,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="2" t="n">
+      <c r="A126" s="1" t="n">
         <v>46031</v>
       </c>
       <c r="B126" t="n">
@@ -4481,7 +4469,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="2" t="n">
+      <c r="A127" s="1" t="n">
         <v>46034</v>
       </c>
       <c r="B127" t="n">
@@ -4513,7 +4501,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="n">
+      <c r="A128" s="1" t="n">
         <v>46038</v>
       </c>
       <c r="B128" t="n">
@@ -4545,7 +4533,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="n">
+      <c r="A129" s="1" t="n">
         <v>46045</v>
       </c>
       <c r="B129" t="n">
@@ -4577,7 +4565,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="n">
+      <c r="A130" s="1" t="n">
         <v>46048</v>
       </c>
       <c r="B130" t="n">
@@ -4609,7 +4597,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="n">
+      <c r="A131" s="1" t="n">
         <v>46052</v>
       </c>
       <c r="B131" t="n">
@@ -4641,7 +4629,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="2" t="n">
+      <c r="A132" s="1" t="n">
         <v>46053</v>
       </c>
       <c r="B132" t="n">
@@ -4673,7 +4661,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="2" t="n">
+      <c r="A133" s="1" t="n">
         <v>46059</v>
       </c>
       <c r="B133" t="n">
@@ -4702,6 +4690,38 @@
       </c>
       <c r="J133" t="n">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>46075</v>
+      </c>
+      <c r="B134" t="n">
+        <v>9</v>
+      </c>
+      <c r="C134" t="n">
+        <v>43.97167851248931</v>
+      </c>
+      <c r="D134" t="n">
+        <v>34.21319262483131</v>
+      </c>
+      <c r="E134" t="n">
+        <v>2.989592657248895</v>
+      </c>
+      <c r="F134" t="n">
+        <v>1.516188619161831</v>
+      </c>
+      <c r="G134" t="n">
+        <v>3.17313512481893</v>
+      </c>
+      <c r="H134" t="n">
+        <v>2.531679534968201</v>
+      </c>
+      <c r="I134" t="n">
+        <v>10.1601723059689</v>
+      </c>
+      <c r="J134" t="n">
+        <v>1.444360620512625</v>
       </c>
     </row>
   </sheetData>
@@ -4724,22 +4744,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>조사기관</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>weight</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>weight_pct</t>
         </is>

</xml_diff>

<commit_message>
chore: hourly poll update (2026-02-23~2026-03-01)
</commit_message>
<xml_diff>
--- a/codex_handoff_pack/outputs/weighted_time_series.xlsx
+++ b/codex_handoff_pack/outputs/weighted_time_series.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4722,6 +4722,38 @@
       </c>
       <c r="J134" t="n">
         <v>2.025203543281836</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>46082</v>
+      </c>
+      <c r="B135" t="n">
+        <v>9</v>
+      </c>
+      <c r="C135" t="n">
+        <v>44.01314686240003</v>
+      </c>
+      <c r="D135" t="n">
+        <v>31.595714368587</v>
+      </c>
+      <c r="E135" t="n">
+        <v>3.965111291106811</v>
+      </c>
+      <c r="F135" t="n">
+        <v>2.649163027124037</v>
+      </c>
+      <c r="G135" t="n">
+        <v>4.348288357026851</v>
+      </c>
+      <c r="H135" t="n">
+        <v>3.35597543423588</v>
+      </c>
+      <c r="I135" t="n">
+        <v>8.473163716677444</v>
+      </c>
+      <c r="J135" t="n">
+        <v>1.599436942841936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>